<commit_message>
Moved all changes from testing to Main Branch
</commit_message>
<xml_diff>
--- a/data/Smart FM Defects through Python.xlsx
+++ b/data/Smart FM Defects through Python.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tabreze\GIT_SmartFM_Replacement_DefectsDashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997113B5-4DC0-4579-9B30-2A8722091E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F60A41D-2F6B-4BE5-8955-32E7F04C2CDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="327">
   <si>
     <t>ID</t>
   </si>
@@ -1001,6 +1001,9 @@
   </si>
   <si>
     <t>https://dev.azure.com/SobhaRealty/OneApp/_workitems/edit/8930</t>
+  </si>
+  <si>
+    <t>Resolved</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1346,7 @@
   <dimension ref="A1:H150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E159" sqref="E159"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2038,7 +2041,7 @@
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>10</v>
+        <v>326</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>

</xml_diff>